<commit_message>
cambiato Ore Totale con Totale
</commit_message>
<xml_diff>
--- a/Esterni/PianoDiProgetto/fileExcel.xlsx
+++ b/Esterni/PianoDiProgetto/fileExcel.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biancaciuche/ProgettoSWEDocumentazione/Esterni/PianoDiProgetto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matteo\Desktop\ZeroSeven\ProgettoSWEDocumentazione\Esterni\PianoDiProgetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC57399-D1D2-7143-A2B6-5748E2A74518}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39576F42-C0B3-4D9E-8EF3-11C7AE318D41}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="760" windowWidth="21420" windowHeight="15540" xr2:uid="{91D0A290-4AC5-3F40-8EB7-44DFE5407311}"/>
+    <workbookView xWindow="4776" yWindow="756" windowWidth="21420" windowHeight="15540" xr2:uid="{91D0A290-4AC5-3F40-8EB7-44DFE5407311}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="36">
   <si>
     <t>Nome</t>
   </si>
@@ -106,9 +112,6 @@
   </si>
   <si>
     <t>Ore totali ruolo</t>
-  </si>
-  <si>
-    <t>Ore totali</t>
   </si>
   <si>
     <t>Analisi dei requisiti in dettaglio</t>
@@ -2733,7 +2736,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1307356335"/>
@@ -2793,7 +2796,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1307393023"/>
@@ -2843,7 +2846,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2873,7 +2876,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3135,7 +3138,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -3378,7 +3381,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -3509,7 +3512,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4135,7 +4138,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1373484687"/>
@@ -4194,7 +4197,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1373137167"/>
@@ -4236,7 +4239,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4273,7 +4276,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4478,7 +4481,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="it-IT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
               <c:showLegendKey val="0"/>
@@ -4590,7 +4593,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -4850,7 +4853,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -4984,7 +4987,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5610,7 +5613,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1371404351"/>
@@ -5669,7 +5672,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1341894079"/>
@@ -5711,7 +5714,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5741,7 +5744,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6022,7 +6025,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -6268,7 +6271,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -6402,7 +6405,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6690,7 +6693,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -6936,7 +6939,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -7070,7 +7073,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7697,7 +7700,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1339571615"/>
@@ -7757,7 +7760,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1337458207"/>
@@ -7807,7 +7810,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7837,7 +7840,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8064,7 +8067,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="it-IT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
               <c:showLegendKey val="0"/>
@@ -8175,7 +8178,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -8421,7 +8424,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -8555,7 +8558,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9112,7 +9115,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1340823151"/>
@@ -9172,7 +9175,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1340547871"/>
@@ -9214,7 +9217,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9244,7 +9247,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9483,7 +9486,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -9743,7 +9746,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -9877,7 +9880,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10452,7 +10455,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1336774463"/>
@@ -10511,7 +10514,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1340163471"/>
@@ -10553,7 +10556,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10583,7 +10586,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10843,7 +10846,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -11103,7 +11106,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -11237,7 +11240,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11863,7 +11866,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1373092639"/>
@@ -11922,7 +11925,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1373087999"/>
@@ -11964,7 +11967,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11994,7 +11997,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -20723,26 +20726,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969318DE-3F76-F04F-8210-53F47E738A81}">
   <dimension ref="A1:V90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:H62"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="7" width="4.83203125" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.19921875" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.296875" customWidth="1"/>
+    <col min="10" max="10" width="15.69921875" customWidth="1"/>
+    <col min="11" max="11" width="13.19921875" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" customWidth="1"/>
-    <col min="20" max="20" width="23.33203125" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" customWidth="1"/>
-    <col min="22" max="22" width="17.83203125" customWidth="1"/>
+    <col min="18" max="18" width="15.19921875" customWidth="1"/>
+    <col min="19" max="19" width="14.296875" customWidth="1"/>
+    <col min="20" max="20" width="23.296875" customWidth="1"/>
+    <col min="21" max="21" width="11.296875" customWidth="1"/>
+    <col min="22" max="22" width="17.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20" customHeight="1">
+    <row r="1" spans="1:22" ht="19.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -20780,7 +20788,7 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:22" ht="20" customHeight="1">
+    <row r="2" spans="1:22" ht="19.95" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -20824,7 +20832,7 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:22" ht="20" customHeight="1">
+    <row r="3" spans="1:22" ht="19.95" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -20868,7 +20876,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="20" customHeight="1">
+    <row r="4" spans="1:22" ht="19.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -20912,7 +20920,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="1:22" ht="20" customHeight="1">
+    <row r="5" spans="1:22" ht="19.95" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -20954,7 +20962,7 @@
       <c r="U5" s="2"/>
       <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="1:22" ht="20" customHeight="1">
+    <row r="6" spans="1:22" ht="19.95" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -20996,7 +21004,7 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:22" ht="20" customHeight="1">
+    <row r="7" spans="1:22" ht="19.95" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -21040,7 +21048,7 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:22" ht="20" customHeight="1">
+    <row r="8" spans="1:22" ht="19.95" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -21067,7 +21075,7 @@
         <v>24</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K8" s="1">
         <v>175</v>
@@ -21082,7 +21090,7 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="20" customHeight="1">
+    <row r="9" spans="1:22" ht="19.95" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -21118,10 +21126,10 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="19" customHeight="1">
+    <row r="13" spans="1:22" ht="19.05" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -21129,13 +21137,13 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -21157,24 +21165,24 @@
       </c>
       <c r="S13" s="2"/>
     </row>
-    <row r="14" spans="1:22" ht="23" customHeight="1">
+    <row r="14" spans="1:22" ht="22.95" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1">
         <v>2</v>
@@ -21197,7 +21205,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="20" customHeight="1">
+    <row r="15" spans="1:22" ht="19.95" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -21205,19 +21213,19 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="1">
         <f>SUM(Tabella1[[#This Row],[Re]:[Ve]])</f>
@@ -21241,24 +21249,24 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="1:22" ht="20" customHeight="1">
+    <row r="16" spans="1:22" ht="19.95" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" s="1">
         <v>3</v>
@@ -21285,24 +21293,24 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="1:22" ht="20" customHeight="1">
+    <row r="17" spans="1:22" ht="19.95" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="1">
         <v>3</v>
@@ -21315,10 +21323,10 @@
         <v>15</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -21327,24 +21335,24 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:22" ht="20" customHeight="1">
+    <row r="18" spans="1:22" ht="19.95" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="1">
         <v>2</v>
@@ -21357,10 +21365,10 @@
         <v>16</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -21369,24 +21377,24 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="1:22" ht="20" customHeight="1">
+    <row r="19" spans="1:22" ht="19.95" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="1">
         <v>3</v>
@@ -21412,24 +21420,24 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="1:22" ht="20" customHeight="1">
+    <row r="20" spans="1:22" ht="19.95" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1">
         <v>3</v>
@@ -21439,7 +21447,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K20" s="1">
         <f>SUM(K14:K19)</f>
@@ -21456,7 +21464,7 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="1:22" ht="20" customHeight="1">
+    <row r="21" spans="1:22" ht="19.95" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
@@ -21472,10 +21480,10 @@
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="1">
         <f>SUM(G14:G20)</f>
@@ -21491,9 +21499,9 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="1:22" ht="20" customHeight="1">
+    <row r="22" spans="1:22" ht="19.95" customHeight="1">
       <c r="J22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -21504,7 +21512,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="20" customHeight="1">
+    <row r="26" spans="1:22" ht="19.95" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -21539,7 +21547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="20" customHeight="1">
+    <row r="27" spans="1:22" ht="19.95" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -21573,7 +21581,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="20" customHeight="1">
+    <row r="28" spans="1:22" ht="19.95" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -21608,7 +21616,7 @@
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
     </row>
-    <row r="29" spans="1:22" ht="20" customHeight="1">
+    <row r="29" spans="1:22" ht="19.95" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -21641,7 +21649,7 @@
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="1:22" ht="20" customHeight="1">
+    <row r="30" spans="1:22" ht="19.95" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -21676,7 +21684,7 @@
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:22" ht="20" customHeight="1">
+    <row r="31" spans="1:22" ht="19.95" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -21711,7 +21719,7 @@
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
     </row>
-    <row r="32" spans="1:22" ht="20" customHeight="1">
+    <row r="32" spans="1:22" ht="19.95" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -21744,7 +21752,7 @@
       <c r="R32" s="2"/>
       <c r="S32" s="4"/>
     </row>
-    <row r="33" spans="1:19" ht="20" customHeight="1">
+    <row r="33" spans="1:19" ht="19.95" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -21763,7 +21771,7 @@
         <v>27</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K33" s="1">
         <f>SUM(K27:K32)</f>
@@ -21777,7 +21785,7 @@
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
     </row>
-    <row r="34" spans="1:19" ht="20" customHeight="1">
+    <row r="34" spans="1:19" ht="19.95" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>26</v>
       </c>
@@ -21813,7 +21821,7 @@
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
     </row>
-    <row r="35" spans="1:19" ht="20" customHeight="1">
+    <row r="35" spans="1:19" ht="19.95" customHeight="1">
       <c r="A35" s="7"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -21826,20 +21834,20 @@
       <c r="R35" s="2"/>
       <c r="S35" s="4"/>
     </row>
-    <row r="36" spans="1:19" ht="20" customHeight="1">
+    <row r="36" spans="1:19" ht="19.95" customHeight="1">
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
     </row>
-    <row r="38" spans="1:19" ht="20" customHeight="1">
+    <row r="38" spans="1:19" ht="19.95" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -21877,7 +21885,7 @@
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
     </row>
-    <row r="39" spans="1:19" ht="20" customHeight="1">
+    <row r="39" spans="1:19" ht="19.95" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
@@ -21909,7 +21917,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="20" customHeight="1">
+    <row r="40" spans="1:19" ht="19.95" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -21943,7 +21951,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="20" customHeight="1">
+    <row r="41" spans="1:19" ht="19.95" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
@@ -21977,7 +21985,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="20" customHeight="1">
+    <row r="42" spans="1:19" ht="19.95" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -22009,7 +22017,7 @@
         <v>2574</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="20" customHeight="1">
+    <row r="43" spans="1:19" ht="19.95" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>6</v>
       </c>
@@ -22046,7 +22054,7 @@
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
     </row>
-    <row r="44" spans="1:19" ht="20" customHeight="1">
+    <row r="44" spans="1:19" ht="19.95" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -22083,7 +22091,7 @@
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
     </row>
-    <row r="45" spans="1:19" ht="20" customHeight="1">
+    <row r="45" spans="1:19" ht="19.95" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -22104,7 +22112,7 @@
         <v>53</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K45" s="1">
         <f>SUM(K39:K44)</f>
@@ -22118,7 +22126,7 @@
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
     </row>
-    <row r="46" spans="1:19" ht="20" customHeight="1">
+    <row r="46" spans="1:19" ht="19.95" customHeight="1">
       <c r="A46" s="7" t="s">
         <v>26</v>
       </c>
@@ -22225,10 +22233,10 @@
     </row>
     <row r="53" spans="1:19">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="20" customHeight="1">
+    <row r="54" spans="1:19" ht="19.95" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -22236,13 +22244,13 @@
         <v>23</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>1</v>
@@ -22263,24 +22271,24 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="20" customHeight="1">
+    <row r="55" spans="1:19" ht="19.95" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E55" s="1">
         <v>9</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G55" s="1">
         <v>12</v>
@@ -22300,24 +22308,24 @@
         <v>360</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="20" customHeight="1">
+    <row r="56" spans="1:19" ht="19.95" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E56" s="1">
         <v>12</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G56" s="1">
         <v>9</v>
@@ -22338,24 +22346,24 @@
         <v>420</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="20" customHeight="1">
+    <row r="57" spans="1:19" ht="19.95" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" s="1">
         <v>8</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G57" s="1">
         <v>13</v>
@@ -22370,7 +22378,7 @@
       <c r="K57" s="1"/>
       <c r="L57" s="8"/>
     </row>
-    <row r="58" spans="1:19" ht="20" customHeight="1">
+    <row r="58" spans="1:19" ht="19.95" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
@@ -22378,16 +22386,16 @@
         <v>6</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G58" s="1">
         <v>14</v>
@@ -22411,24 +22419,24 @@
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
     </row>
-    <row r="59" spans="1:19" ht="20" customHeight="1">
+    <row r="59" spans="1:19" ht="19.95" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C59" s="1">
         <v>9</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G59" s="1">
         <v>13</v>
@@ -22452,7 +22460,7 @@
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
     </row>
-    <row r="60" spans="1:19" ht="20" customHeight="1">
+    <row r="60" spans="1:19" ht="19.95" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -22460,10 +22468,10 @@
         <v>6</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60" s="1">
         <v>3</v>
@@ -22472,7 +22480,7 @@
         <v>11</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H60" s="1">
         <f>SUM(Tabella13481034613[[#This Row],[Re]:[Ve]])</f>
@@ -22493,21 +22501,21 @@
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
     </row>
-    <row r="61" spans="1:19" ht="20" customHeight="1">
+    <row r="61" spans="1:19" ht="19.95" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C61" s="1">
         <v>4</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F61" s="1">
         <v>14</v>
@@ -22520,7 +22528,7 @@
         <v>21</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K61" s="1">
         <f>SUM(K55:K60)</f>
@@ -22534,7 +22542,7 @@
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
     </row>
-    <row r="62" spans="1:19" ht="20" customHeight="1">
+    <row r="62" spans="1:19" ht="19.95" customHeight="1">
       <c r="A62" s="7" t="s">
         <v>26</v>
       </c>
@@ -22547,7 +22555,7 @@
         <v>21</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E62" s="1">
         <f>SUM(E55:E61)</f>
@@ -22610,10 +22618,10 @@
     </row>
     <row r="68" spans="1:19">
       <c r="A68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="20" customHeight="1">
+    <row r="70" spans="1:19" ht="19.95" customHeight="1">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -22648,15 +22656,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="20" customHeight="1">
+    <row r="71" spans="1:19" ht="19.95" customHeight="1">
       <c r="A71" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D71" s="1">
         <v>14</v>
@@ -22689,12 +22697,12 @@
         <v>960</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="20" customHeight="1">
+    <row r="72" spans="1:19" ht="19.95" customHeight="1">
       <c r="A72" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C72" s="1">
         <f t="shared" ref="C72:C78" si="8">SUM(C56,C40,C28)</f>
@@ -22732,7 +22740,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="20" customHeight="1">
+    <row r="73" spans="1:19" ht="19.95" customHeight="1">
       <c r="A73" s="1" t="s">
         <v>4</v>
       </c>
@@ -22776,7 +22784,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="20" customHeight="1">
+    <row r="74" spans="1:19" ht="19.95" customHeight="1">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
@@ -22785,7 +22793,7 @@
         <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D74" s="1">
         <f t="shared" si="9"/>
@@ -22819,7 +22827,7 @@
         <v>5368</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="20" customHeight="1">
+    <row r="75" spans="1:19" ht="19.95" customHeight="1">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -22832,7 +22840,7 @@
         <v>14</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E75" s="1">
         <f t="shared" si="5"/>
@@ -22862,7 +22870,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="20" customHeight="1">
+    <row r="76" spans="1:19" ht="19.95" customHeight="1">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -22875,7 +22883,7 @@
         <v>6</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E76" s="1">
         <f t="shared" si="5"/>
@@ -22905,7 +22913,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="20" customHeight="1">
+    <row r="77" spans="1:19" ht="19.95" customHeight="1">
       <c r="A77" s="1" t="s">
         <v>8</v>
       </c>
@@ -22918,7 +22926,7 @@
         <v>4</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E77" s="1">
         <f t="shared" si="5"/>
@@ -22937,7 +22945,7 @@
         <v>101</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K77" s="1">
         <f>SUM(K71:K76)</f>
@@ -22948,7 +22956,7 @@
         <v>13268</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="20" customHeight="1">
+    <row r="78" spans="1:19" ht="19.95" customHeight="1">
       <c r="A78" s="7" t="s">
         <v>26</v>
       </c>
@@ -23003,7 +23011,7 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -23013,7 +23021,7 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="20" customHeight="1">
+    <row r="82" spans="1:12" ht="19.95" customHeight="1">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -23048,7 +23056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="20" customHeight="1">
+    <row r="83" spans="1:12" ht="19.95" customHeight="1">
       <c r="A83" s="1" t="s">
         <v>2</v>
       </c>
@@ -23092,7 +23100,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="20" customHeight="1">
+    <row r="84" spans="1:12" ht="19.95" customHeight="1">
       <c r="A84" s="1" t="s">
         <v>3</v>
       </c>
@@ -23136,7 +23144,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="20" customHeight="1">
+    <row r="85" spans="1:12" ht="19.95" customHeight="1">
       <c r="A85" s="1" t="s">
         <v>4</v>
       </c>
@@ -23180,7 +23188,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="20" customHeight="1">
+    <row r="86" spans="1:12" ht="19.95" customHeight="1">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -23224,7 +23232,7 @@
         <v>5368</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="20" customHeight="1">
+    <row r="87" spans="1:12" ht="19.95" customHeight="1">
       <c r="A87" s="1" t="s">
         <v>6</v>
       </c>
@@ -23268,7 +23276,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="20" customHeight="1">
+    <row r="88" spans="1:12" ht="19.95" customHeight="1">
       <c r="A88" s="1" t="s">
         <v>7</v>
       </c>
@@ -23312,7 +23320,7 @@
         <v>3645</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="20" customHeight="1">
+    <row r="89" spans="1:12" ht="19.95" customHeight="1">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
@@ -23345,7 +23353,7 @@
         <v>130</v>
       </c>
       <c r="J89" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K89" s="1">
         <f>SUM(K83:K88)</f>
@@ -23356,7 +23364,7 @@
         <v>17608</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="20" customHeight="1">
+    <row r="90" spans="1:12" ht="19.95" customHeight="1">
       <c r="A90" s="7" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
modifica di alcuni dati eaggiunte
</commit_message>
<xml_diff>
--- a/Esterni/PianoDiProgetto/fileExcel.xlsx
+++ b/Esterni/PianoDiProgetto/fileExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matteo\Desktop\ZeroSeven\ProgettoSWEDocumentazione\Esterni\PianoDiProgetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39576F42-C0B3-4D9E-8EF3-11C7AE318D41}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B08E1F3-B66B-4491-BB08-23F5025860C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4776" yWindow="756" windowWidth="21420" windowHeight="15540" xr2:uid="{91D0A290-4AC5-3F40-8EB7-44DFE5407311}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="36">
   <si>
     <t>Nome</t>
   </si>
@@ -145,7 +145,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +185,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,6 +240,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -8240,7 +8249,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8500,7 +8509,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>165</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20726,8 +20735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969318DE-3F76-F04F-8210-53F47E738A81}">
   <dimension ref="A1:V90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -20950,6 +20959,7 @@
         <v>15</v>
       </c>
       <c r="K5" s="1">
+        <f>E9</f>
         <v>0</v>
       </c>
       <c r="L5" s="1">
@@ -20992,6 +21002,7 @@
         <v>16</v>
       </c>
       <c r="K6" s="1">
+        <f>F9</f>
         <v>0</v>
       </c>
       <c r="L6" s="1">
@@ -21078,10 +21089,12 @@
         <v>13</v>
       </c>
       <c r="K8" s="1">
-        <v>175</v>
-      </c>
-      <c r="L8" s="8">
-        <v>3845</v>
+        <f>SUM(K2:K7)</f>
+        <v>168</v>
+      </c>
+      <c r="L8" s="1">
+        <f>SUM(L2:L7)</f>
+        <v>3625</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="2"/>
@@ -21322,8 +21335,9 @@
       <c r="J17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>30</v>
+      <c r="K17" s="1" t="str">
+        <f>E21</f>
+        <v>-</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>30</v>
@@ -21364,8 +21378,9 @@
       <c r="J18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>30</v>
+      <c r="K18" s="1" t="str">
+        <f>F21</f>
+        <v>-</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>30</v>
@@ -21407,11 +21422,12 @@
         <v>12</v>
       </c>
       <c r="K19" s="1">
-        <v>11</v>
+        <f>G21</f>
+        <v>16</v>
       </c>
       <c r="L19" s="1">
         <f>Tabella3714[[#This Row],[Ore]]*15</f>
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -21450,12 +21466,12 @@
         <v>13</v>
       </c>
       <c r="K20" s="1">
-        <f>SUM(K14:K19)</f>
-        <v>30</v>
+        <f>H21</f>
+        <v>35</v>
       </c>
       <c r="L20" s="1">
         <f>SUM(L14:L19)</f>
-        <v>640</v>
+        <v>715</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -21490,6 +21506,7 @@
         <v>16</v>
       </c>
       <c r="H21" s="1">
+        <f>SUM(H14:H20)</f>
         <v>35</v>
       </c>
       <c r="Q21" s="6"/>
@@ -21817,6 +21834,7 @@
         <f t="shared" si="1"/>
         <v>197</v>
       </c>
+      <c r="I34" s="9"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
@@ -23399,10 +23417,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="14">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -23416,6 +23433,7 @@
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>